<commit_message>
Update wapo metadaten about missing data in March
</commit_message>
<xml_diff>
--- a/automation/wapo_wetterstationen/Metadaten_wetterstationen_my.xlsx
+++ b/automation/wapo_wetterstationen/Metadaten_wetterstationen_my.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\OGD\Daten\Quelldaten\SID\WAPO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\dev\opendatazurich.github.io\automation\wapo_wetterstationen\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD52B7F-028B-4DF5-9A90-B4630D04C50D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="-50" windowWidth="21230" windowHeight="12540"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="14" r:id="rId1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="225">
   <si>
     <t>Erstmalige Veröffentlichung</t>
   </si>
@@ -529,9 +530,6 @@
     <t>Messwerte der Wetterstationen der Wasserschutzpolizei Zürich</t>
   </si>
   <si>
-    <t>Weitere Informationen:</t>
-  </si>
-  <si>
     <t>Luftfeuchte (%): Ist das Verhältnis der aktuellen Wasserdampfmenge in der Luft zur maximal aufnehmbaren, bei der gerade herrschenden Temperatur.</t>
   </si>
   <si>
@@ -617,9 +615,6 @@
   </si>
   <si>
     <t>Anzeige der Messwerte:</t>
-  </si>
-  <si>
-    <t>Historisierte Messwerte seit 2007</t>
   </si>
   <si>
     <t>ressourcen</t>
@@ -686,12 +681,6 @@
     <t>Wenn Sie direkt mit den Messdaten (aktuelles und vorheriges Jahr) der beiden Wetterstationen arbeiten möchten, können Sie die von **Stefan Oderbolz** aus Eigeninitiative privat entwickelte REST-API namens [**Tecdottir**](https://data.stadt-zuerich.ch/showcase/wetterstation-api) verwenden. Dieses ermöglicht ein einfaches abfragen und exportieren der Messdaten als JSON-Datei.</t>
   </si>
   <si>
-    <t>Die historisierten Messwertdaten (10 minütige Frequenz) seit 2007 - Vorjahr stehen nicht via Webseite oder API zur Verfügung, sondern können hier als csv-Dateien herunter geladen werden. Diese Zeitreihen stehen pro Messstation zur Verfügung.</t>
-  </si>
-  <si>
-    <t>Unter folgendem Link ist eine [**Bedienungsanleitung**](https://www.tecson-data.ch/zurich/seepozh/bedienanleitung.pdf) zu finden.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Die beiden Wetterstationen **Tiefenbrunnen** (beim Dienstgebäude der Wasserpolizei) und **Mythenquai** (Hafen Enge) liefern Messwerte sowohl zu aktuellen wie auch zu vergangenen Wettersituationen (aktuelles und vorheriges Jahr). Über die REST-API namens [**Tecdottir**](https://data.stadt-zuerich.ch/showcase/wetterstation-api) können diese Daten direkt bezogen werden.
 Die älteren Daten können als csv-Dateien herunter geladen werden.
 Die Messwerte umfassen: Lufttemperatur, Luftfeuchte, Luftdruck, Taupunkt, Wassertemperatur, Windböen, Windgeschwindigkeit, Windstärke, Windrichtung und Windchill. Zusätzlich liefert die Wetterstation Mythenquai noch die Messwerte zu Globalstrahlung, Niederschlagsmenge und dem Pegelstand des Zürichsees.
@@ -711,11 +700,17 @@
 Bei der Zeitumstellung im Frühling fehlt jeweils die Stunde zwischen 02:00-03:00 Uhr, d.h. auf die Messung von 01:50 Uhr folgt die Messung von 03:00 Uhr.
 Im Herbst wird bei der Zeitumstellung systembedingt jeweils nur eine Messung pro Zeitangabe zwischen 02:00-03:00 Uhr übermittelt, d.h. die Stunde 01:00-02:00 UTC fehlt in den Daten.</t>
   </si>
+  <si>
+    <t>Datenlücke im März 2023</t>
+  </si>
+  <si>
+    <t>Vom 28.2. bis 21.3.2023 fehlen die Wetterdaten in den CSV Dateien. Diese wurden in diesem Zeitraum leider nicht zur Verfügung gestellt.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -1127,9 +1122,9 @@
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Standard 2" xfId="1"/>
-    <cellStyle name="Standard 3" xfId="2"/>
-    <cellStyle name="Standard 4" xfId="3"/>
+    <cellStyle name="Standard 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Standard 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Standard 4" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1370,26 +1365,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G59"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="255.5" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="255.5" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.08203125" style="18" customWidth="1"/>
+    <col min="1" max="1" width="21.125" style="18" customWidth="1"/>
     <col min="2" max="2" width="31.5" style="6" customWidth="1"/>
     <col min="3" max="3" width="64.25" style="6" customWidth="1"/>
-    <col min="4" max="4" width="61.08203125" style="7" customWidth="1"/>
-    <col min="5" max="5" width="17.83203125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="88.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="61.125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="17.875" style="7" customWidth="1"/>
+    <col min="6" max="6" width="88.875" style="1" customWidth="1"/>
     <col min="7" max="7" width="66.5" style="1" customWidth="1"/>
     <col min="8" max="16384" width="255.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
         <v>30</v>
       </c>
@@ -1412,7 +1407,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="6" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="6" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
         <v>31</v>
       </c>
@@ -1433,7 +1428,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="6" customFormat="1" ht="163.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" s="6" customFormat="1" ht="163.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
         <v>92</v>
       </c>
@@ -1444,7 +1439,7 @@
         <v>20</v>
       </c>
       <c r="D3" s="50" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="E3" s="43"/>
       <c r="F3" s="11" t="s">
@@ -1454,7 +1449,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="6" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" s="6" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
         <v>32</v>
       </c>
@@ -1475,7 +1470,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
         <v>33</v>
       </c>
@@ -1492,7 +1487,7 @@
       </c>
       <c r="G5" s="10"/>
     </row>
-    <row r="6" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
         <v>35</v>
       </c>
@@ -1513,7 +1508,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="6" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" s="6" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
         <v>47</v>
       </c>
@@ -1534,7 +1529,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="s">
         <v>48</v>
       </c>
@@ -1555,7 +1550,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="s">
         <v>49</v>
       </c>
@@ -1566,7 +1561,7 @@
         <v>20</v>
       </c>
       <c r="D9" s="39" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E9" s="44"/>
       <c r="F9" s="10" t="s">
@@ -1576,7 +1571,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="6" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A10" s="18" t="s">
         <v>50</v>
       </c>
@@ -1587,7 +1582,7 @@
         <v>21</v>
       </c>
       <c r="D10" s="38" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E10" s="43"/>
       <c r="F10" s="10" t="s">
@@ -1597,7 +1592,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="18" t="s">
         <v>51</v>
       </c>
@@ -1608,7 +1603,7 @@
         <v>21</v>
       </c>
       <c r="D11" s="40" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E11" s="14" t="s">
         <v>148</v>
@@ -1620,7 +1615,7 @@
         <v>41823</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="18" t="s">
         <v>52</v>
       </c>
@@ -1641,7 +1636,7 @@
         <v>41823</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="18" t="s">
         <v>54</v>
       </c>
@@ -1659,7 +1654,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="18" t="s">
         <v>55</v>
       </c>
@@ -1680,7 +1675,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="6" customFormat="1" ht="25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" s="6" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A15" s="18" t="s">
         <v>84</v>
       </c>
@@ -1691,7 +1686,7 @@
         <v>21</v>
       </c>
       <c r="D15" s="39" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E15" s="44"/>
       <c r="F15" s="10" t="s">
@@ -1701,7 +1696,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="18" t="s">
         <v>89</v>
       </c>
@@ -1722,22 +1717,22 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="B17" s="34" t="s">
         <v>195</v>
-      </c>
-      <c r="B17" s="34" t="s">
-        <v>196</v>
       </c>
       <c r="C17" s="37"/>
       <c r="D17" s="46" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E17" s="46"/>
       <c r="F17" s="10"/>
       <c r="G17" s="21"/>
     </row>
-    <row r="18" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="18"/>
       <c r="B18" s="5"/>
       <c r="C18" s="10"/>
@@ -1745,7 +1740,7 @@
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="18" t="s">
         <v>53</v>
       </c>
@@ -1758,7 +1753,7 @@
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B20" s="33" t="s">
         <v>13</v>
       </c>
@@ -1772,148 +1767,153 @@
         <v>87</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="62.5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A21" s="18" t="s">
         <v>88</v>
       </c>
       <c r="B21" s="31" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C21" s="38" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D21" s="31"/>
       <c r="E21" s="47"/>
     </row>
-    <row r="22" spans="1:7" ht="212.5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="216.75" x14ac:dyDescent="0.2">
       <c r="A22" s="18" t="s">
         <v>88</v>
       </c>
       <c r="B22" s="31" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C22" s="38" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D22" s="31"/>
       <c r="E22" s="47"/>
     </row>
-    <row r="23" spans="1:7" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A23" s="18" t="s">
         <v>88</v>
       </c>
       <c r="B23" s="31" t="s">
-        <v>199</v>
+        <v>223</v>
       </c>
       <c r="C23" s="38" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="D23" s="31"/>
       <c r="E23" s="47"/>
     </row>
-    <row r="24" spans="1:7" ht="25" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A24" s="18" t="s">
         <v>88</v>
       </c>
       <c r="B24" s="32" t="s">
-        <v>169</v>
-      </c>
-      <c r="C24" s="39" t="s">
-        <v>221</v>
+        <v>219</v>
+      </c>
+      <c r="C24" s="38" t="s">
+        <v>222</v>
       </c>
       <c r="D24" s="32"/>
       <c r="E24" s="48"/>
     </row>
-    <row r="25" spans="1:7" ht="112.5" x14ac:dyDescent="0.3">
-      <c r="A25" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="B25" s="32" t="s">
-        <v>223</v>
-      </c>
-      <c r="C25" s="38" t="s">
-        <v>226</v>
-      </c>
-      <c r="D25" s="32"/>
-      <c r="E25" s="48"/>
-    </row>
-    <row r="26" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A26" s="18"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="10"/>
-    </row>
-    <row r="27" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A27" s="18" t="s">
+    <row r="25" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A25" s="18"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="10"/>
+    </row>
+    <row r="26" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A26" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B26" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C26" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12" t="s">
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A28" s="18"/>
-      <c r="B28" s="33" t="s">
+    <row r="27" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A27" s="18"/>
+      <c r="B27" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="C28" s="33" t="s">
+      <c r="C27" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="D28" s="33" t="s">
+      <c r="D27" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="E28" s="33"/>
-      <c r="F28" s="6" t="s">
+      <c r="E27" s="33"/>
+      <c r="F27" s="6" t="s">
         <v>76</v>
       </c>
+      <c r="G27" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A28" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" s="49" t="s">
+        <v>180</v>
+      </c>
+      <c r="C28" s="49" t="s">
+        <v>213</v>
+      </c>
+      <c r="D28" s="49" t="s">
+        <v>220</v>
+      </c>
+      <c r="E28" s="47"/>
       <c r="G28" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" s="6" customFormat="1" ht="39" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A29" s="18" t="s">
         <v>42</v>
       </c>
       <c r="B29" s="49" t="s">
-        <v>181</v>
+        <v>214</v>
       </c>
       <c r="C29" s="49" t="s">
         <v>215</v>
       </c>
       <c r="D29" s="49" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E29" s="47"/>
-      <c r="G29" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" s="6" customFormat="1" ht="39" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="18" t="s">
         <v>42</v>
       </c>
       <c r="B30" s="49" t="s">
-        <v>216</v>
+        <v>181</v>
       </c>
       <c r="C30" s="49" t="s">
-        <v>217</v>
+        <v>151</v>
       </c>
       <c r="D30" s="49" t="s">
-        <v>225</v>
-      </c>
-      <c r="E30" s="47"/>
-    </row>
-    <row r="31" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+      <c r="E30" s="48"/>
+      <c r="G30" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A31" s="18" t="s">
         <v>42</v>
       </c>
@@ -1921,17 +1921,17 @@
         <v>182</v>
       </c>
       <c r="C31" s="49" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D31" s="49" t="s">
-        <v>175</v>
+        <v>211</v>
       </c>
       <c r="E31" s="48"/>
       <c r="G31" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" s="6" customFormat="1" ht="39" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" s="6" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A32" s="18" t="s">
         <v>42</v>
       </c>
@@ -1939,17 +1939,14 @@
         <v>183</v>
       </c>
       <c r="C32" s="49" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D32" s="49" t="s">
-        <v>213</v>
+        <v>172</v>
       </c>
       <c r="E32" s="48"/>
-      <c r="G32" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" s="6" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:7" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A33" s="18" t="s">
         <v>42</v>
       </c>
@@ -1957,14 +1954,14 @@
         <v>184</v>
       </c>
       <c r="C33" s="49" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D33" s="49" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="E33" s="48"/>
     </row>
-    <row r="34" spans="1:5" s="6" customFormat="1" ht="39" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="18" t="s">
         <v>42</v>
       </c>
@@ -1972,14 +1969,14 @@
         <v>185</v>
       </c>
       <c r="C34" s="49" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D34" s="49" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E34" s="48"/>
     </row>
-    <row r="35" spans="1:5" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" s="6" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A35" s="18" t="s">
         <v>42</v>
       </c>
@@ -1987,14 +1984,14 @@
         <v>186</v>
       </c>
       <c r="C35" s="49" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D35" s="49" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E35" s="48"/>
     </row>
-    <row r="36" spans="1:5" s="6" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" s="6" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A36" s="18" t="s">
         <v>42</v>
       </c>
@@ -2002,14 +1999,14 @@
         <v>187</v>
       </c>
       <c r="C36" s="49" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D36" s="49" t="s">
-        <v>172</v>
-      </c>
-      <c r="E36" s="48"/>
-    </row>
-    <row r="37" spans="1:5" s="6" customFormat="1" ht="65" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+      <c r="E36" s="47"/>
+    </row>
+    <row r="37" spans="1:7" s="6" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A37" s="18" t="s">
         <v>42</v>
       </c>
@@ -2017,14 +2014,14 @@
         <v>188</v>
       </c>
       <c r="C37" s="49" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D37" s="49" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="E37" s="47"/>
     </row>
-    <row r="38" spans="1:5" s="6" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A38" s="18" t="s">
         <v>42</v>
       </c>
@@ -2032,14 +2029,14 @@
         <v>189</v>
       </c>
       <c r="C38" s="49" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D38" s="49" t="s">
-        <v>171</v>
+        <v>208</v>
       </c>
       <c r="E38" s="47"/>
     </row>
-    <row r="39" spans="1:5" s="6" customFormat="1" ht="39" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" s="6" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A39" s="18" t="s">
         <v>42</v>
       </c>
@@ -2047,14 +2044,14 @@
         <v>190</v>
       </c>
       <c r="C39" s="49" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D39" s="49" t="s">
-        <v>210</v>
+        <v>177</v>
       </c>
       <c r="E39" s="47"/>
     </row>
-    <row r="40" spans="1:5" s="6" customFormat="1" ht="52" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A40" s="18" t="s">
         <v>42</v>
       </c>
@@ -2062,14 +2059,14 @@
         <v>191</v>
       </c>
       <c r="C40" s="49" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D40" s="49" t="s">
-        <v>178</v>
+        <v>209</v>
       </c>
       <c r="E40" s="47"/>
     </row>
-    <row r="41" spans="1:5" s="6" customFormat="1" ht="39" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A41" s="18" t="s">
         <v>42</v>
       </c>
@@ -2077,14 +2074,14 @@
         <v>192</v>
       </c>
       <c r="C41" s="49" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D41" s="49" t="s">
-        <v>211</v>
+        <v>169</v>
       </c>
       <c r="E41" s="47"/>
     </row>
-    <row r="42" spans="1:5" s="6" customFormat="1" ht="39" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" s="6" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A42" s="18" t="s">
         <v>42</v>
       </c>
@@ -2092,122 +2089,115 @@
         <v>193</v>
       </c>
       <c r="C42" s="49" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D42" s="49" t="s">
-        <v>170</v>
+        <v>210</v>
       </c>
       <c r="E42" s="47"/>
     </row>
-    <row r="43" spans="1:5" s="6" customFormat="1" ht="26" x14ac:dyDescent="0.3">
-      <c r="A43" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="B43" s="49" t="s">
-        <v>194</v>
-      </c>
-      <c r="C43" s="49" t="s">
-        <v>163</v>
-      </c>
-      <c r="D43" s="49" t="s">
-        <v>212</v>
-      </c>
-      <c r="E43" s="47"/>
-    </row>
-    <row r="44" spans="1:5" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A43" s="18"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+    </row>
+    <row r="44" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="18"/>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
       <c r="D44" s="10"/>
       <c r="E44" s="10"/>
     </row>
-    <row r="45" spans="1:5" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="18"/>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
       <c r="D45" s="10"/>
       <c r="E45" s="10"/>
     </row>
-    <row r="46" spans="1:5" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="18"/>
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
-      <c r="D46" s="10"/>
-      <c r="E46" s="10"/>
-    </row>
-    <row r="47" spans="1:5" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A47" s="18"/>
-      <c r="B47" s="5"/>
-      <c r="C47" s="5"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
+    </row>
+    <row r="47" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A47" s="18" t="s">
+        <v>198</v>
+      </c>
+      <c r="B47" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>21</v>
+      </c>
       <c r="D47" s="9"/>
       <c r="E47" s="9"/>
     </row>
-    <row r="48" spans="1:5" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A48" s="18" t="s">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B48" s="33" t="s">
         <v>200</v>
       </c>
-      <c r="B48" s="12" t="s">
+      <c r="C48" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="D48" s="33"/>
+      <c r="E48" s="33"/>
+      <c r="F48" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="G48" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A49" s="18" t="s">
+        <v>199</v>
+      </c>
+      <c r="B49" s="31" t="s">
         <v>202</v>
       </c>
-      <c r="C48" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D48" s="9"/>
-      <c r="E48" s="9"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B49" s="33" t="s">
-        <v>202</v>
-      </c>
-      <c r="C49" s="33" t="s">
-        <v>92</v>
-      </c>
-      <c r="D49" s="33"/>
-      <c r="E49" s="33"/>
-      <c r="F49" s="3" t="s">
+      <c r="C49" s="31" t="s">
         <v>203</v>
       </c>
-      <c r="G49" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.3">
+      <c r="D49" s="31"/>
+      <c r="E49" s="47"/>
+      <c r="F49" s="10"/>
+    </row>
+    <row r="50" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="18" t="s">
-        <v>201</v>
-      </c>
-      <c r="B50" s="31" t="s">
+        <v>199</v>
+      </c>
+      <c r="B50" s="32" t="s">
+        <v>205</v>
+      </c>
+      <c r="C50" s="31" t="s">
         <v>204</v>
       </c>
-      <c r="C50" s="31" t="s">
-        <v>205</v>
-      </c>
-      <c r="D50" s="31"/>
-      <c r="E50" s="47"/>
+      <c r="D50" s="32"/>
+      <c r="E50" s="48"/>
       <c r="F50" s="10"/>
     </row>
-    <row r="51" spans="1:7" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.3">
-      <c r="A51" s="18" t="s">
-        <v>201</v>
-      </c>
-      <c r="B51" s="32" t="s">
-        <v>207</v>
-      </c>
-      <c r="C51" s="31" t="s">
-        <v>206</v>
-      </c>
+    <row r="51" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A51" s="18"/>
+      <c r="B51" s="32"/>
+      <c r="C51" s="32"/>
       <c r="D51" s="32"/>
       <c r="E51" s="48"/>
       <c r="F51" s="10"/>
     </row>
-    <row r="52" spans="1:7" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="18"/>
-      <c r="B52" s="32"/>
-      <c r="C52" s="32"/>
-      <c r="D52" s="32"/>
-      <c r="E52" s="48"/>
+      <c r="B52" s="15"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="10"/>
+      <c r="E52" s="10"/>
       <c r="F52" s="10"/>
     </row>
-    <row r="53" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="18"/>
       <c r="B53" s="15"/>
       <c r="C53" s="10"/>
@@ -2215,75 +2205,67 @@
       <c r="E53" s="10"/>
       <c r="F53" s="10"/>
     </row>
-    <row r="54" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A54" s="18"/>
-      <c r="B54" s="15"/>
-      <c r="C54" s="10"/>
+    <row r="54" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A54" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B54" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C54" s="12" t="s">
+        <v>21</v>
+      </c>
       <c r="D54" s="10"/>
       <c r="E54" s="10"/>
       <c r="F54" s="10"/>
     </row>
-    <row r="55" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A55" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="B55" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C55" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D55" s="10"/>
-      <c r="E55" s="10"/>
-      <c r="F55" s="10"/>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B56" s="33" t="s">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B55" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="C56" s="33" t="s">
+      <c r="C55" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="D56" s="33" t="s">
+      <c r="D55" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="E56" s="33"/>
+      <c r="E55" s="33"/>
+      <c r="F55" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G55" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A56" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B56" s="31"/>
+      <c r="C56" s="31"/>
+      <c r="D56" s="31"/>
+      <c r="E56" s="47"/>
       <c r="F56" s="3" t="s">
-        <v>78</v>
+        <v>127</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A57" s="18" t="s">
-        <v>44</v>
-      </c>
+        <v>149</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B57" s="31"/>
       <c r="C57" s="31"/>
       <c r="D57" s="31"/>
       <c r="E57" s="47"/>
-      <c r="F57" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="G57" s="6" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G57" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B58" s="31"/>
       <c r="C58" s="31"/>
       <c r="D58" s="31"/>
       <c r="E58" s="47"/>
-      <c r="G58" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B59" s="31"/>
-      <c r="C59" s="31"/>
-      <c r="D59" s="31"/>
-      <c r="E59" s="47"/>
     </row>
   </sheetData>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.98425196850393704" bottom="0.59055118110236227" header="0.39370078740157483" footer="0.27559055118110237"/>
@@ -2292,25 +2274,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.08203125" style="18" customWidth="1"/>
-    <col min="2" max="2" width="27.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.125" style="18" customWidth="1"/>
+    <col min="2" max="2" width="27.375" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.5" style="6" customWidth="1"/>
-    <col min="4" max="4" width="255.58203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="255.625" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="59" style="3" customWidth="1"/>
     <col min="6" max="6" width="48.75" style="1" customWidth="1"/>
     <col min="7" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
         <v>30</v>
       </c>
@@ -2333,7 +2315,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="6" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="6" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
         <v>31</v>
       </c>
@@ -2353,7 +2335,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="6" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" s="6" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
         <v>92</v>
       </c>
@@ -2373,7 +2355,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="6" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" s="6" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
         <v>32</v>
       </c>
@@ -2393,7 +2375,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
         <v>33</v>
       </c>
@@ -2409,7 +2391,7 @@
       </c>
       <c r="G5" s="10"/>
     </row>
-    <row r="6" spans="1:7" s="6" customFormat="1" ht="25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" s="6" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
         <v>35</v>
       </c>
@@ -2429,7 +2411,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="6" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" s="6" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
         <v>47</v>
       </c>
@@ -2449,7 +2431,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="s">
         <v>48</v>
       </c>
@@ -2469,7 +2451,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="s">
         <v>49</v>
       </c>
@@ -2489,7 +2471,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="18" t="s">
         <v>50</v>
       </c>
@@ -2509,7 +2491,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="18" t="s">
         <v>51</v>
       </c>
@@ -2529,7 +2511,7 @@
         <v>41823</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="18" t="s">
         <v>52</v>
       </c>
@@ -2549,7 +2531,7 @@
         <v>41823</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="18" t="s">
         <v>54</v>
       </c>
@@ -2566,7 +2548,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="18" t="s">
         <v>55</v>
       </c>
@@ -2586,7 +2568,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="18" t="s">
         <v>84</v>
       </c>
@@ -2606,7 +2588,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="18" t="s">
         <v>89</v>
       </c>
@@ -2626,14 +2608,14 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="18"/>
       <c r="B17" s="5"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="F17" s="10"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="18" t="s">
         <v>53</v>
       </c>
@@ -2645,7 +2627,7 @@
       </c>
       <c r="D18" s="9"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B19" s="16" t="s">
         <v>13</v>
       </c>
@@ -2659,7 +2641,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="18" t="s">
         <v>88</v>
       </c>
@@ -2672,7 +2654,7 @@
       <c r="D20" s="29"/>
       <c r="E20" s="20"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="18" t="s">
         <v>88</v>
       </c>
@@ -2685,7 +2667,7 @@
       <c r="D21" s="29"/>
       <c r="E21" s="20"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="18" t="s">
         <v>88</v>
       </c>
@@ -2698,7 +2680,7 @@
       <c r="D22" s="29"/>
       <c r="E22" s="20"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="18" t="s">
         <v>88</v>
       </c>
@@ -2711,14 +2693,14 @@
       <c r="D23" s="29"/>
       <c r="E23" s="20"/>
     </row>
-    <row r="24" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="18"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="F24" s="10"/>
     </row>
-    <row r="25" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="18" t="s">
         <v>41</v>
       </c>
@@ -2733,7 +2715,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="18"/>
       <c r="B26" s="16" t="s">
         <v>38</v>
@@ -2751,7 +2733,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="18" t="s">
         <v>42</v>
       </c>
@@ -2768,7 +2750,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="28" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="18" t="s">
         <v>42</v>
       </c>
@@ -2785,7 +2767,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="18" t="s">
         <v>42</v>
       </c>
@@ -2802,7 +2784,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="18" t="s">
         <v>42</v>
       </c>
@@ -2819,7 +2801,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="18" t="s">
         <v>42</v>
       </c>
@@ -2836,7 +2818,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="18" t="s">
         <v>42</v>
       </c>
@@ -2850,7 +2832,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="33" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="18" t="s">
         <v>42</v>
       </c>
@@ -2864,7 +2846,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="34" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="18" t="s">
         <v>42</v>
       </c>
@@ -2878,7 +2860,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="35" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="18" t="s">
         <v>42</v>
       </c>
@@ -2892,31 +2874,31 @@
         <v>120</v>
       </c>
     </row>
-    <row r="36" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="18"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="10"/>
     </row>
-    <row r="37" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="18"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
       <c r="D37" s="10"/>
     </row>
-    <row r="38" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="18"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="10"/>
     </row>
-    <row r="39" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="18"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="9"/>
     </row>
-    <row r="40" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="18" t="s">
         <v>45</v>
       </c>
@@ -2928,7 +2910,7 @@
       </c>
       <c r="D40" s="9"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B41" s="16" t="s">
         <v>13</v>
       </c>
@@ -2945,7 +2927,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="18" t="s">
         <v>46</v>
       </c>
@@ -2961,7 +2943,7 @@
       <c r="F42" s="3"/>
       <c r="G42" s="6"/>
     </row>
-    <row r="43" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="18" t="s">
         <v>46</v>
       </c>
@@ -2976,7 +2958,7 @@
       </c>
       <c r="F43" s="10"/>
     </row>
-    <row r="44" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="18" t="s">
         <v>46</v>
       </c>
@@ -2991,7 +2973,7 @@
       </c>
       <c r="F44" s="10"/>
     </row>
-    <row r="45" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="18" t="s">
         <v>46</v>
       </c>
@@ -3006,21 +2988,21 @@
       </c>
       <c r="F45" s="10"/>
     </row>
-    <row r="46" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="18"/>
       <c r="B46" s="15"/>
       <c r="C46" s="10"/>
       <c r="D46" s="10"/>
       <c r="F46" s="10"/>
     </row>
-    <row r="47" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="18"/>
       <c r="B47" s="15"/>
       <c r="C47" s="10"/>
       <c r="D47" s="10"/>
       <c r="F47" s="10"/>
     </row>
-    <row r="48" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="18" t="s">
         <v>43</v>
       </c>
@@ -3033,7 +3015,7 @@
       <c r="D48" s="10"/>
       <c r="F48" s="10"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B49" s="16" t="s">
         <v>13</v>
       </c>
@@ -3050,7 +3032,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="18" t="s">
         <v>44</v>
       </c>
@@ -3189,18 +3171,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3220,6 +3202,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4B3AD83-9986-4E71-995F-A94C1CED6EB8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6056489-A7A4-4445-AFC5-87E5586E5E93}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -3232,12 +3222,4 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4B3AD83-9986-4E71-995F-A94C1CED6EB8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add remark about missing data
</commit_message>
<xml_diff>
--- a/automation/wapo_wetterstationen/Metadaten_wetterstationen_my.xlsx
+++ b/automation/wapo_wetterstationen/Metadaten_wetterstationen_my.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\dev\opendatazurich.github.io\automation\wapo_wetterstationen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD52B7F-028B-4DF5-9A90-B4630D04C50D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B055CFF4-C93D-400B-B5CE-C12C5DA0EFBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="14" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="223">
   <si>
     <t>Erstmalige Veröffentlichung</t>
   </si>
@@ -614,9 +614,6 @@
     <t>22.04.2007 - aktuell</t>
   </si>
   <si>
-    <t>Anzeige der Messwerte:</t>
-  </si>
-  <si>
     <t>ressourcen</t>
   </si>
   <si>
@@ -669,16 +666,6 @@
   </si>
   <si>
     <t>Datum / Uhrzeit (UTC)</t>
-  </si>
-  <si>
-    <t>Die Messwertdaten können nicht direkt von der Webseite der Messstationen als Datei herunter geladen, sondern als HTML-Tabelle angezeigt werden. 
-Sie können über die folgenden Links die gewünschte Wetterstation, den Zeitraum und die Messwerte auswählen, welche als HTML-Tabelle ausgegeben werden sollen. Dabei können Sie auch noch auswählen, ob Sie sich nur Tagesdurschnittswerte oder alle Werte (10 minütige Frequenz) anzeigen lassen möchten. 
--  [Wetterstation **Mythenquai**](https://www.tecson-data.ch/zurich/mythenquai/index.php)
-- [Wetterstation **Tiefenbrunnen**](https://www.tecson-data.ch/zurich/tiefenbrunnen/index.php)
-Wenn Sie auf einer der beiden Webseite sind, klicken Sie bitte unten auf **Anzeige aller Messerte**. Danach erscheinen die Funktionalitäten um manuell die gewünschten Daten und Messwerte auszuwählen und anzeigen zu lassen.</t>
-  </si>
-  <si>
-    <t>Wenn Sie direkt mit den Messdaten (aktuelles und vorheriges Jahr) der beiden Wetterstationen arbeiten möchten, können Sie die von **Stefan Oderbolz** aus Eigeninitiative privat entwickelte REST-API namens [**Tecdottir**](https://data.stadt-zuerich.ch/showcase/wetterstation-api) verwenden. Dieses ermöglicht ein einfaches abfragen und exportieren der Messdaten als JSON-Datei.</t>
   </si>
   <si>
     <t xml:space="preserve">Die beiden Wetterstationen **Tiefenbrunnen** (beim Dienstgebäude der Wasserpolizei) und **Mythenquai** (Hafen Enge) liefern Messwerte sowohl zu aktuellen wie auch zu vergangenen Wettersituationen (aktuelles und vorheriges Jahr). Über die REST-API namens [**Tecdottir**](https://data.stadt-zuerich.ch/showcase/wetterstation-api) können diese Daten direkt bezogen werden.
@@ -701,10 +688,13 @@
 Im Herbst wird bei der Zeitumstellung systembedingt jeweils nur eine Messung pro Zeitangabe zwischen 02:00-03:00 Uhr übermittelt, d.h. die Stunde 01:00-02:00 UTC fehlt in den Daten.</t>
   </si>
   <si>
-    <t>Datenlücke im März 2023</t>
-  </si>
-  <si>
-    <t>Vom 28.2. bis 21.3.2023 fehlen die Wetterdaten in den CSV Dateien. Diese wurden in diesem Zeitraum leider nicht zur Verfügung gestellt.</t>
+    <t>Fehlende Daten</t>
+  </si>
+  <si>
+    <t>Wenn Sie direkt mit den Messdaten der beiden Wetterstationen arbeiten möchten, können Sie die von **Stefan Oderbolz** aus Eigeninitiative privat entwickelte REST-API namens [**Tecdottir**](https://data.stadt-zuerich.ch/showcase/wetterstation-api) verwenden. Dieses ermöglicht ein einfaches abfragen und exportieren der Messdaten als JSON-Datei.</t>
+  </si>
+  <si>
+    <t>Bis auf weiteres werden diese Daten nicht aktualisiert, da diese nicht mehr zur Verfügung gestellt werden. Bitte wenden Sie sich direkt an die Wasserschutzpolizei, um diese Daten zu beziehen ([wasserschutz@zuerich.ch](mailto:wasserschutz@zuerich.ch)).</t>
   </si>
 </sst>
 </file>
@@ -1366,25 +1356,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G58"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="255.5" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="255.5" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.125" style="18" customWidth="1"/>
+    <col min="1" max="1" width="21.08203125" style="18" customWidth="1"/>
     <col min="2" max="2" width="31.5" style="6" customWidth="1"/>
     <col min="3" max="3" width="64.25" style="6" customWidth="1"/>
-    <col min="4" max="4" width="61.125" style="7" customWidth="1"/>
-    <col min="5" max="5" width="17.875" style="7" customWidth="1"/>
-    <col min="6" max="6" width="88.875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="61.08203125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="17.83203125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="88.83203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="66.5" style="1" customWidth="1"/>
     <col min="8" max="16384" width="255.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>30</v>
       </c>
@@ -1407,7 +1397,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="6" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" s="6" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>31</v>
       </c>
@@ -1428,7 +1418,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="6" customFormat="1" ht="163.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" s="6" customFormat="1" ht="163.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>92</v>
       </c>
@@ -1439,7 +1429,7 @@
         <v>20</v>
       </c>
       <c r="D3" s="50" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E3" s="43"/>
       <c r="F3" s="11" t="s">
@@ -1449,7 +1439,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="6" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" s="6" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>32</v>
       </c>
@@ -1470,7 +1460,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>33</v>
       </c>
@@ -1487,7 +1477,7 @@
       </c>
       <c r="G5" s="10"/>
     </row>
-    <row r="6" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>35</v>
       </c>
@@ -1508,7 +1498,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="6" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" s="6" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
         <v>47</v>
       </c>
@@ -1529,7 +1519,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
         <v>48</v>
       </c>
@@ -1550,7 +1540,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
         <v>49</v>
       </c>
@@ -1571,7 +1561,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" s="6" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
         <v>50</v>
       </c>
@@ -1582,7 +1572,7 @@
         <v>21</v>
       </c>
       <c r="D10" s="38" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E10" s="43"/>
       <c r="F10" s="10" t="s">
@@ -1592,7 +1582,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
         <v>51</v>
       </c>
@@ -1603,7 +1593,7 @@
         <v>21</v>
       </c>
       <c r="D11" s="40" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E11" s="14" t="s">
         <v>148</v>
@@ -1615,7 +1605,7 @@
         <v>41823</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
         <v>52</v>
       </c>
@@ -1636,7 +1626,7 @@
         <v>41823</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
         <v>54</v>
       </c>
@@ -1654,7 +1644,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
         <v>55</v>
       </c>
@@ -1675,7 +1665,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="6" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" s="6" customFormat="1" ht="25" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
         <v>84</v>
       </c>
@@ -1696,7 +1686,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A16" s="18" t="s">
         <v>89</v>
       </c>
@@ -1717,7 +1707,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A17" s="18" t="s">
         <v>194</v>
       </c>
@@ -1726,13 +1716,13 @@
       </c>
       <c r="C17" s="37"/>
       <c r="D17" s="46" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E17" s="46"/>
       <c r="F17" s="10"/>
       <c r="G17" s="21"/>
     </row>
-    <row r="18" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A18" s="18"/>
       <c r="B18" s="5"/>
       <c r="C18" s="10"/>
@@ -1740,7 +1730,7 @@
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="18" t="s">
         <v>53</v>
       </c>
@@ -1753,7 +1743,7 @@
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B20" s="33" t="s">
         <v>13</v>
       </c>
@@ -1767,429 +1757,424 @@
         <v>87</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="50" x14ac:dyDescent="0.3">
       <c r="A21" s="18" t="s">
         <v>88</v>
       </c>
       <c r="B21" s="31" t="s">
-        <v>179</v>
+        <v>220</v>
       </c>
       <c r="C21" s="38" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="D21" s="31"/>
       <c r="E21" s="47"/>
     </row>
-    <row r="22" spans="1:7" ht="216.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="62.5" x14ac:dyDescent="0.3">
       <c r="A22" s="18" t="s">
         <v>88</v>
       </c>
       <c r="B22" s="31" t="s">
-        <v>197</v>
+        <v>179</v>
       </c>
       <c r="C22" s="38" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="D22" s="31"/>
       <c r="E22" s="47"/>
     </row>
-    <row r="23" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="112.5" x14ac:dyDescent="0.3">
       <c r="A23" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="B23" s="31" t="s">
-        <v>223</v>
+      <c r="B23" s="32" t="s">
+        <v>216</v>
       </c>
       <c r="C23" s="38" t="s">
-        <v>224</v>
-      </c>
-      <c r="D23" s="31"/>
-      <c r="E23" s="47"/>
-    </row>
-    <row r="24" spans="1:7" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A24" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="B24" s="32" t="s">
         <v>219</v>
       </c>
-      <c r="C24" s="38" t="s">
-        <v>222</v>
-      </c>
-      <c r="D24" s="32"/>
-      <c r="E24" s="48"/>
-    </row>
-    <row r="25" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="18"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="10"/>
-    </row>
-    <row r="26" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="18" t="s">
+      <c r="D23" s="32"/>
+      <c r="E23" s="48"/>
+    </row>
+    <row r="24" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+      <c r="A24" s="18"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="10"/>
+    </row>
+    <row r="25" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+      <c r="A25" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="B25" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C25" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12" t="s">
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="18"/>
-      <c r="B27" s="33" t="s">
+    <row r="26" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+      <c r="A26" s="18"/>
+      <c r="B26" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="33" t="s">
+      <c r="C26" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="D27" s="33" t="s">
+      <c r="D26" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="E27" s="33"/>
-      <c r="F27" s="6" t="s">
+      <c r="E26" s="33"/>
+      <c r="F26" s="6" t="s">
         <v>76</v>
       </c>
+      <c r="G26" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" s="6" customFormat="1" ht="39" x14ac:dyDescent="0.3">
+      <c r="A27" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" s="49" t="s">
+        <v>180</v>
+      </c>
+      <c r="C27" s="49" t="s">
+        <v>212</v>
+      </c>
+      <c r="D27" s="49" t="s">
+        <v>217</v>
+      </c>
+      <c r="E27" s="47"/>
       <c r="G27" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" s="6" customFormat="1" ht="39" x14ac:dyDescent="0.3">
       <c r="A28" s="18" t="s">
         <v>42</v>
       </c>
       <c r="B28" s="49" t="s">
-        <v>180</v>
+        <v>213</v>
       </c>
       <c r="C28" s="49" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D28" s="49" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E28" s="47"/>
-      <c r="G28" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A29" s="18" t="s">
         <v>42</v>
       </c>
       <c r="B29" s="49" t="s">
-        <v>214</v>
+        <v>181</v>
       </c>
       <c r="C29" s="49" t="s">
-        <v>215</v>
+        <v>151</v>
       </c>
       <c r="D29" s="49" t="s">
-        <v>221</v>
-      </c>
-      <c r="E29" s="47"/>
-    </row>
-    <row r="30" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+        <v>174</v>
+      </c>
+      <c r="E29" s="48"/>
+      <c r="G29" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" s="6" customFormat="1" ht="39" x14ac:dyDescent="0.3">
       <c r="A30" s="18" t="s">
         <v>42</v>
       </c>
       <c r="B30" s="49" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C30" s="49" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D30" s="49" t="s">
-        <v>174</v>
+        <v>210</v>
       </c>
       <c r="E30" s="48"/>
       <c r="G30" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" s="6" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A31" s="18" t="s">
         <v>42</v>
       </c>
       <c r="B31" s="49" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C31" s="49" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D31" s="49" t="s">
-        <v>211</v>
+        <v>172</v>
       </c>
       <c r="E31" s="48"/>
-      <c r="G31" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" s="6" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:7" s="6" customFormat="1" ht="39" x14ac:dyDescent="0.3">
       <c r="A32" s="18" t="s">
         <v>42</v>
       </c>
       <c r="B32" s="49" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C32" s="49" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D32" s="49" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="E32" s="48"/>
     </row>
-    <row r="33" spans="1:7" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A33" s="18" t="s">
         <v>42</v>
       </c>
       <c r="B33" s="49" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C33" s="49" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D33" s="49" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E33" s="48"/>
     </row>
-    <row r="34" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" s="6" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A34" s="18" t="s">
         <v>42</v>
       </c>
       <c r="B34" s="49" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C34" s="49" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D34" s="49" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E34" s="48"/>
     </row>
-    <row r="35" spans="1:7" s="6" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" s="6" customFormat="1" ht="65" x14ac:dyDescent="0.3">
       <c r="A35" s="18" t="s">
         <v>42</v>
       </c>
       <c r="B35" s="49" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C35" s="49" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D35" s="49" t="s">
-        <v>171</v>
-      </c>
-      <c r="E35" s="48"/>
-    </row>
-    <row r="36" spans="1:7" s="6" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+        <v>176</v>
+      </c>
+      <c r="E35" s="47"/>
+    </row>
+    <row r="36" spans="1:7" s="6" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A36" s="18" t="s">
         <v>42</v>
       </c>
       <c r="B36" s="49" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C36" s="49" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D36" s="49" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="E36" s="47"/>
     </row>
-    <row r="37" spans="1:7" s="6" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" s="6" customFormat="1" ht="39" x14ac:dyDescent="0.3">
       <c r="A37" s="18" t="s">
         <v>42</v>
       </c>
       <c r="B37" s="49" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C37" s="49" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D37" s="49" t="s">
-        <v>170</v>
+        <v>207</v>
       </c>
       <c r="E37" s="47"/>
     </row>
-    <row r="38" spans="1:7" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" s="6" customFormat="1" ht="52" x14ac:dyDescent="0.3">
       <c r="A38" s="18" t="s">
         <v>42</v>
       </c>
       <c r="B38" s="49" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C38" s="49" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D38" s="49" t="s">
-        <v>208</v>
+        <v>177</v>
       </c>
       <c r="E38" s="47"/>
     </row>
-    <row r="39" spans="1:7" s="6" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" s="6" customFormat="1" ht="39" x14ac:dyDescent="0.3">
       <c r="A39" s="18" t="s">
         <v>42</v>
       </c>
       <c r="B39" s="49" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C39" s="49" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D39" s="49" t="s">
-        <v>177</v>
+        <v>208</v>
       </c>
       <c r="E39" s="47"/>
     </row>
-    <row r="40" spans="1:7" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" s="6" customFormat="1" ht="39" x14ac:dyDescent="0.3">
       <c r="A40" s="18" t="s">
         <v>42</v>
       </c>
       <c r="B40" s="49" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C40" s="49" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D40" s="49" t="s">
-        <v>209</v>
+        <v>169</v>
       </c>
       <c r="E40" s="47"/>
     </row>
-    <row r="41" spans="1:7" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" s="6" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A41" s="18" t="s">
         <v>42</v>
       </c>
       <c r="B41" s="49" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C41" s="49" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D41" s="49" t="s">
-        <v>169</v>
+        <v>209</v>
       </c>
       <c r="E41" s="47"/>
     </row>
-    <row r="42" spans="1:7" s="6" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A42" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="B42" s="49" t="s">
-        <v>193</v>
-      </c>
-      <c r="C42" s="49" t="s">
-        <v>163</v>
-      </c>
-      <c r="D42" s="49" t="s">
-        <v>210</v>
-      </c>
-      <c r="E42" s="47"/>
-    </row>
-    <row r="43" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+      <c r="A42" s="18"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+    </row>
+    <row r="43" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A43" s="18"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
       <c r="D43" s="10"/>
       <c r="E43" s="10"/>
     </row>
-    <row r="44" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A44" s="18"/>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
       <c r="D44" s="10"/>
       <c r="E44" s="10"/>
     </row>
-    <row r="45" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A45" s="18"/>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
-      <c r="D45" s="10"/>
-      <c r="E45" s="10"/>
-    </row>
-    <row r="46" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A46" s="18"/>
-      <c r="B46" s="5"/>
-      <c r="C46" s="5"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="9"/>
+    </row>
+    <row r="46" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+      <c r="A46" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="C46" s="12" t="s">
+        <v>21</v>
+      </c>
       <c r="D46" s="9"/>
       <c r="E46" s="9"/>
     </row>
-    <row r="47" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A47" s="18" t="s">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B47" s="33" t="s">
+        <v>199</v>
+      </c>
+      <c r="C47" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="D47" s="33"/>
+      <c r="E47" s="33"/>
+      <c r="F47" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="G47" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.3">
+      <c r="A48" s="18" t="s">
         <v>198</v>
       </c>
-      <c r="B47" s="12" t="s">
-        <v>200</v>
-      </c>
-      <c r="C47" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D47" s="9"/>
-      <c r="E47" s="9"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B48" s="33" t="s">
-        <v>200</v>
-      </c>
-      <c r="C48" s="33" t="s">
-        <v>92</v>
-      </c>
-      <c r="D48" s="33"/>
-      <c r="E48" s="33"/>
-      <c r="F48" s="3" t="s">
+      <c r="B48" s="31" t="s">
         <v>201</v>
       </c>
-      <c r="G48" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C48" s="31" t="s">
+        <v>202</v>
+      </c>
+      <c r="D48" s="31"/>
+      <c r="E48" s="47"/>
+      <c r="F48" s="10"/>
+    </row>
+    <row r="49" spans="1:7" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.3">
       <c r="A49" s="18" t="s">
-        <v>199</v>
-      </c>
-      <c r="B49" s="31" t="s">
-        <v>202</v>
+        <v>198</v>
+      </c>
+      <c r="B49" s="32" t="s">
+        <v>204</v>
       </c>
       <c r="C49" s="31" t="s">
         <v>203</v>
       </c>
-      <c r="D49" s="31"/>
-      <c r="E49" s="47"/>
+      <c r="D49" s="32"/>
+      <c r="E49" s="48"/>
       <c r="F49" s="10"/>
     </row>
-    <row r="50" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A50" s="18" t="s">
-        <v>199</v>
-      </c>
-      <c r="B50" s="32" t="s">
-        <v>205</v>
-      </c>
-      <c r="C50" s="31" t="s">
-        <v>204</v>
-      </c>
+    <row r="50" spans="1:7" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.3">
+      <c r="A50" s="18"/>
+      <c r="B50" s="32"/>
+      <c r="C50" s="32"/>
       <c r="D50" s="32"/>
       <c r="E50" s="48"/>
       <c r="F50" s="10"/>
     </row>
-    <row r="51" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A51" s="18"/>
-      <c r="B51" s="32"/>
-      <c r="C51" s="32"/>
-      <c r="D51" s="32"/>
-      <c r="E51" s="48"/>
+      <c r="B51" s="15"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="10"/>
+      <c r="E51" s="10"/>
       <c r="F51" s="10"/>
     </row>
-    <row r="52" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A52" s="18"/>
       <c r="B52" s="15"/>
       <c r="C52" s="10"/>
@@ -2197,75 +2182,67 @@
       <c r="E52" s="10"/>
       <c r="F52" s="10"/>
     </row>
-    <row r="53" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A53" s="18"/>
-      <c r="B53" s="15"/>
-      <c r="C53" s="10"/>
+    <row r="53" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+      <c r="A53" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B53" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C53" s="12" t="s">
+        <v>21</v>
+      </c>
       <c r="D53" s="10"/>
       <c r="E53" s="10"/>
       <c r="F53" s="10"/>
     </row>
-    <row r="54" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A54" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="B54" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C54" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D54" s="10"/>
-      <c r="E54" s="10"/>
-      <c r="F54" s="10"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B55" s="33" t="s">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B54" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="C55" s="33" t="s">
+      <c r="C54" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="D55" s="33" t="s">
+      <c r="D54" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="E55" s="33"/>
+      <c r="E54" s="33"/>
+      <c r="F54" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G54" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A55" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B55" s="31"/>
+      <c r="C55" s="31"/>
+      <c r="D55" s="31"/>
+      <c r="E55" s="47"/>
       <c r="F55" s="3" t="s">
-        <v>78</v>
+        <v>127</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A56" s="18" t="s">
-        <v>44</v>
-      </c>
+        <v>149</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B56" s="31"/>
       <c r="C56" s="31"/>
       <c r="D56" s="31"/>
       <c r="E56" s="47"/>
-      <c r="F56" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="G56" s="6" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G56" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B57" s="31"/>
       <c r="C57" s="31"/>
       <c r="D57" s="31"/>
       <c r="E57" s="47"/>
-      <c r="G57" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B58" s="31"/>
-      <c r="C58" s="31"/>
-      <c r="D58" s="31"/>
-      <c r="E58" s="47"/>
     </row>
   </sheetData>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.98425196850393704" bottom="0.59055118110236227" header="0.39370078740157483" footer="0.27559055118110237"/>
@@ -2281,18 +2258,18 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.125" style="18" customWidth="1"/>
-    <col min="2" max="2" width="27.375" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.08203125" style="18" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.5" style="6" customWidth="1"/>
-    <col min="4" max="4" width="255.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="255.58203125" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="59" style="3" customWidth="1"/>
     <col min="6" max="6" width="48.75" style="1" customWidth="1"/>
     <col min="7" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>30</v>
       </c>
@@ -2315,7 +2292,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="6" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" s="6" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>31</v>
       </c>
@@ -2335,7 +2312,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="6" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" s="6" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>92</v>
       </c>
@@ -2355,7 +2332,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="6" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" s="6" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>32</v>
       </c>
@@ -2375,7 +2352,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>33</v>
       </c>
@@ -2391,7 +2368,7 @@
       </c>
       <c r="G5" s="10"/>
     </row>
-    <row r="6" spans="1:7" s="6" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" s="6" customFormat="1" ht="25" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>35</v>
       </c>
@@ -2411,7 +2388,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="6" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" s="6" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
         <v>47</v>
       </c>
@@ -2431,7 +2408,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
         <v>48</v>
       </c>
@@ -2451,7 +2428,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
         <v>49</v>
       </c>
@@ -2471,7 +2448,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
         <v>50</v>
       </c>
@@ -2491,7 +2468,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
         <v>51</v>
       </c>
@@ -2511,7 +2488,7 @@
         <v>41823</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
         <v>52</v>
       </c>
@@ -2531,7 +2508,7 @@
         <v>41823</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
         <v>54</v>
       </c>
@@ -2548,7 +2525,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
         <v>55</v>
       </c>
@@ -2568,7 +2545,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
         <v>84</v>
       </c>
@@ -2588,7 +2565,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A16" s="18" t="s">
         <v>89</v>
       </c>
@@ -2608,14 +2585,14 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A17" s="18"/>
       <c r="B17" s="5"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="F17" s="10"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="18" t="s">
         <v>53</v>
       </c>
@@ -2627,7 +2604,7 @@
       </c>
       <c r="D18" s="9"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B19" s="16" t="s">
         <v>13</v>
       </c>
@@ -2641,7 +2618,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="18" t="s">
         <v>88</v>
       </c>
@@ -2654,7 +2631,7 @@
       <c r="D20" s="29"/>
       <c r="E20" s="20"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="18" t="s">
         <v>88</v>
       </c>
@@ -2667,7 +2644,7 @@
       <c r="D21" s="29"/>
       <c r="E21" s="20"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="18" t="s">
         <v>88</v>
       </c>
@@ -2680,7 +2657,7 @@
       <c r="D22" s="29"/>
       <c r="E22" s="20"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="18" t="s">
         <v>88</v>
       </c>
@@ -2693,14 +2670,14 @@
       <c r="D23" s="29"/>
       <c r="E23" s="20"/>
     </row>
-    <row r="24" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A24" s="18"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="F24" s="10"/>
     </row>
-    <row r="25" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A25" s="18" t="s">
         <v>41</v>
       </c>
@@ -2715,7 +2692,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A26" s="18"/>
       <c r="B26" s="16" t="s">
         <v>38</v>
@@ -2733,7 +2710,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A27" s="18" t="s">
         <v>42</v>
       </c>
@@ -2750,7 +2727,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="28" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A28" s="18" t="s">
         <v>42</v>
       </c>
@@ -2767,7 +2744,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A29" s="18" t="s">
         <v>42</v>
       </c>
@@ -2784,7 +2761,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A30" s="18" t="s">
         <v>42</v>
       </c>
@@ -2801,7 +2778,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A31" s="18" t="s">
         <v>42</v>
       </c>
@@ -2818,7 +2795,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A32" s="18" t="s">
         <v>42</v>
       </c>
@@ -2832,7 +2809,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="33" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A33" s="18" t="s">
         <v>42</v>
       </c>
@@ -2846,7 +2823,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="34" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A34" s="18" t="s">
         <v>42</v>
       </c>
@@ -2860,7 +2837,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="35" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A35" s="18" t="s">
         <v>42</v>
       </c>
@@ -2874,31 +2851,31 @@
         <v>120</v>
       </c>
     </row>
-    <row r="36" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A36" s="18"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="10"/>
     </row>
-    <row r="37" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A37" s="18"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
       <c r="D37" s="10"/>
     </row>
-    <row r="38" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A38" s="18"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="10"/>
     </row>
-    <row r="39" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A39" s="18"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="9"/>
     </row>
-    <row r="40" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A40" s="18" t="s">
         <v>45</v>
       </c>
@@ -2910,7 +2887,7 @@
       </c>
       <c r="D40" s="9"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B41" s="16" t="s">
         <v>13</v>
       </c>
@@ -2927,7 +2904,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="18" t="s">
         <v>46</v>
       </c>
@@ -2943,7 +2920,7 @@
       <c r="F42" s="3"/>
       <c r="G42" s="6"/>
     </row>
-    <row r="43" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A43" s="18" t="s">
         <v>46</v>
       </c>
@@ -2958,7 +2935,7 @@
       </c>
       <c r="F43" s="10"/>
     </row>
-    <row r="44" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A44" s="18" t="s">
         <v>46</v>
       </c>
@@ -2973,7 +2950,7 @@
       </c>
       <c r="F44" s="10"/>
     </row>
-    <row r="45" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A45" s="18" t="s">
         <v>46</v>
       </c>
@@ -2988,21 +2965,21 @@
       </c>
       <c r="F45" s="10"/>
     </row>
-    <row r="46" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A46" s="18"/>
       <c r="B46" s="15"/>
       <c r="C46" s="10"/>
       <c r="D46" s="10"/>
       <c r="F46" s="10"/>
     </row>
-    <row r="47" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A47" s="18"/>
       <c r="B47" s="15"/>
       <c r="C47" s="10"/>
       <c r="D47" s="10"/>
       <c r="F47" s="10"/>
     </row>
-    <row r="48" spans="1:7" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A48" s="18" t="s">
         <v>43</v>
       </c>
@@ -3015,7 +2992,7 @@
       <c r="D48" s="10"/>
       <c r="F48" s="10"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B49" s="16" t="s">
         <v>13</v>
       </c>
@@ -3032,7 +3009,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="18" t="s">
         <v>44</v>
       </c>
@@ -3171,18 +3148,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3202,14 +3179,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4B3AD83-9986-4E71-995F-A94C1CED6EB8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6056489-A7A4-4445-AFC5-87E5586E5E93}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -3222,4 +3191,12 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4B3AD83-9986-4E71-995F-A94C1CED6EB8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add note at the beginning
</commit_message>
<xml_diff>
--- a/automation/wapo_wetterstationen/Metadaten_wetterstationen_my.xlsx
+++ b/automation/wapo_wetterstationen/Metadaten_wetterstationen_my.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\dev\opendatazurich.github.io\automation\wapo_wetterstationen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B055CFF4-C93D-400B-B5CE-C12C5DA0EFBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74B154D9-ADDA-4C64-975A-4AFDB44D3AFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -668,33 +668,34 @@
     <t>Datum / Uhrzeit (UTC)</t>
   </si>
   <si>
-    <t xml:space="preserve">Die beiden Wetterstationen **Tiefenbrunnen** (beim Dienstgebäude der Wasserpolizei) und **Mythenquai** (Hafen Enge) liefern Messwerte sowohl zu aktuellen wie auch zu vergangenen Wettersituationen (aktuelles und vorheriges Jahr). Über die REST-API namens [**Tecdottir**](https://data.stadt-zuerich.ch/showcase/wetterstation-api) können diese Daten direkt bezogen werden.
+    <t>Zeitzonen und Zeitumstellung</t>
+  </si>
+  <si>
+    <t>Datum / Uhrzeit in der Mitteleuropäischen Zeit (MEZ) resp. Mitteleuropäischer Sommerzeit (MESZ). Dies entspricht der Lokalzeit für die Messungen. Das Datumsformat entspricht ISO 8601.</t>
+  </si>
+  <si>
+    <t>Datum / Uhrzeit in UTC (koordinierte Weltzeit). Diese Zeitangaben sind von der Lokalzeit umgerechnet und lassen sich ggf. einfacher weiterverarbeiten.  Das Datumsformat entspricht ISO 8601.</t>
+  </si>
+  <si>
+    <t>In diesem Datensatz sind die Zeitangaben sowohl in MEZ/MESZ (Mitteleuropäische Zeit) wie auch in UTC (koordinierte Weltzeit) angegeben. Das Datumsformat entspricht jeweils [ISO 8601](https://de.wikipedia.org/wiki/ISO_8601).
+Bei der Zeitumstellung im Frühling fehlt jeweils die Stunde zwischen 02:00-03:00 Uhr, d.h. auf die Messung von 01:50 Uhr folgt die Messung von 03:00 Uhr.
+Im Herbst wird bei der Zeitumstellung systembedingt jeweils nur eine Messung pro Zeitangabe zwischen 02:00-03:00 Uhr übermittelt, d.h. die Stunde 01:00-02:00 UTC fehlt in den Daten.</t>
+  </si>
+  <si>
+    <t>Fehlende Daten</t>
+  </si>
+  <si>
+    <t>Wenn Sie direkt mit den Messdaten der beiden Wetterstationen arbeiten möchten, können Sie die von **Stefan Oderbolz** aus Eigeninitiative privat entwickelte REST-API namens [**Tecdottir**](https://data.stadt-zuerich.ch/showcase/wetterstation-api) verwenden. Dieses ermöglicht ein einfaches abfragen und exportieren der Messdaten als JSON-Datei.</t>
+  </si>
+  <si>
+    <t>Bis auf weiteres werden diese Daten nicht aktualisiert, da diese nicht mehr zur Verfügung gestellt werden. Bitte wenden Sie sich direkt an die Wasserschutzpolizei, um diese Daten zu beziehen ([wasserschutz@zuerich.ch](mailto:wasserschutz@zuerich.ch)).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**ACHTUNG:** Aktuell können die Daten der Wetterstationen nicht aktualisiert werden, da diese Daten derzeit nicht zur Verfügung stehen. Bitte wenden Sie sich direkt an die Wasserschutzpolizei, um diese Daten zu beziehen ([**wasserschutz@zuerich.ch**](mailto:wasserschutz@zuerich.ch)).
+Die beiden Wetterstationen **Tiefenbrunnen** (beim Dienstgebäude der Wasserpolizei) und **Mythenquai** (Hafen Enge) liefern Messwerte sowohl zu aktuellen wie auch zu vergangenen Wettersituationen. Über die REST-API namens [**Tecdottir**](https://data.stadt-zuerich.ch/showcase/wetterstation-api) können diese Daten direkt bezogen werden.
 Die älteren Daten können als csv-Dateien herunter geladen werden.
 Die Messwerte umfassen: Lufttemperatur, Luftfeuchte, Luftdruck, Taupunkt, Wassertemperatur, Windböen, Windgeschwindigkeit, Windstärke, Windrichtung und Windchill. Zusätzlich liefert die Wetterstation Mythenquai noch die Messwerte zu Globalstrahlung, Niederschlagsmenge und dem Pegelstand des Zürichsees.
 </t>
-  </si>
-  <si>
-    <t>Zeitzonen und Zeitumstellung</t>
-  </si>
-  <si>
-    <t>Datum / Uhrzeit in der Mitteleuropäischen Zeit (MEZ) resp. Mitteleuropäischer Sommerzeit (MESZ). Dies entspricht der Lokalzeit für die Messungen. Das Datumsformat entspricht ISO 8601.</t>
-  </si>
-  <si>
-    <t>Datum / Uhrzeit in UTC (koordinierte Weltzeit). Diese Zeitangaben sind von der Lokalzeit umgerechnet und lassen sich ggf. einfacher weiterverarbeiten.  Das Datumsformat entspricht ISO 8601.</t>
-  </si>
-  <si>
-    <t>In diesem Datensatz sind die Zeitangaben sowohl in MEZ/MESZ (Mitteleuropäische Zeit) wie auch in UTC (koordinierte Weltzeit) angegeben. Das Datumsformat entspricht jeweils [ISO 8601](https://de.wikipedia.org/wiki/ISO_8601).
-Bei der Zeitumstellung im Frühling fehlt jeweils die Stunde zwischen 02:00-03:00 Uhr, d.h. auf die Messung von 01:50 Uhr folgt die Messung von 03:00 Uhr.
-Im Herbst wird bei der Zeitumstellung systembedingt jeweils nur eine Messung pro Zeitangabe zwischen 02:00-03:00 Uhr übermittelt, d.h. die Stunde 01:00-02:00 UTC fehlt in den Daten.</t>
-  </si>
-  <si>
-    <t>Fehlende Daten</t>
-  </si>
-  <si>
-    <t>Wenn Sie direkt mit den Messdaten der beiden Wetterstationen arbeiten möchten, können Sie die von **Stefan Oderbolz** aus Eigeninitiative privat entwickelte REST-API namens [**Tecdottir**](https://data.stadt-zuerich.ch/showcase/wetterstation-api) verwenden. Dieses ermöglicht ein einfaches abfragen und exportieren der Messdaten als JSON-Datei.</t>
-  </si>
-  <si>
-    <t>Bis auf weiteres werden diese Daten nicht aktualisiert, da diese nicht mehr zur Verfügung gestellt werden. Bitte wenden Sie sich direkt an die Wasserschutzpolizei, um diese Daten zu beziehen ([wasserschutz@zuerich.ch](mailto:wasserschutz@zuerich.ch)).</t>
   </si>
 </sst>
 </file>
@@ -1359,7 +1360,7 @@
   <dimension ref="A1:G57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="255.5" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1429,7 +1430,7 @@
         <v>20</v>
       </c>
       <c r="D3" s="50" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="E3" s="43"/>
       <c r="F3" s="11" t="s">
@@ -1762,10 +1763,10 @@
         <v>88</v>
       </c>
       <c r="B21" s="31" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C21" s="38" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D21" s="31"/>
       <c r="E21" s="47"/>
@@ -1778,7 +1779,7 @@
         <v>179</v>
       </c>
       <c r="C22" s="38" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D22" s="31"/>
       <c r="E22" s="47"/>
@@ -1788,10 +1789,10 @@
         <v>88</v>
       </c>
       <c r="B23" s="32" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C23" s="38" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D23" s="32"/>
       <c r="E23" s="48"/>
@@ -1850,7 +1851,7 @@
         <v>212</v>
       </c>
       <c r="D27" s="49" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E27" s="47"/>
       <c r="G27" s="6" t="s">
@@ -1868,7 +1869,7 @@
         <v>214</v>
       </c>
       <c r="D28" s="49" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E28" s="47"/>
     </row>
@@ -3148,18 +3149,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3179,6 +3180,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4B3AD83-9986-4E71-995F-A94C1CED6EB8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6056489-A7A4-4445-AFC5-87E5586E5E93}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -3191,12 +3200,4 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4B3AD83-9986-4E71-995F-A94C1CED6EB8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>